<commit_message>
added support for oee data
</commit_message>
<xml_diff>
--- a/Config/machines_config.xlsx
+++ b/Config/machines_config.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F7FDF36-A764-4515-BBC6-5D4A44DDD526}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\proj_tesi_backend\Config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949C2360-E8F4-452C-9AF2-77388ABC2A26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>nome</t>
   </si>
@@ -37,13 +42,22 @@
   </si>
   <si>
     <t>OP60</t>
+  </si>
+  <si>
+    <t>Machine 1</t>
+  </si>
+  <si>
+    <t>Machine 2</t>
+  </si>
+  <si>
+    <t>Machine 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,7 +115,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -397,18 +411,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,7 +431,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -425,12 +439,36 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>